<commit_message>
Update homeless population by Age.xlsx
</commit_message>
<xml_diff>
--- a/Data/homeless population by Age.xlsx
+++ b/Data/homeless population by Age.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/Data Scientist Program/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/GitHub/Homelessness-Final-Group-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{398C646E-F77F-4368-B52A-2D7771340409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{398C646E-F77F-4368-B52A-2D7771340409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BEAE789-B1D8-4E7F-8B97-CBE3537A1F0D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B9B7E66-A1B9-4B24-A9D4-EC74981F3731}"/>
   </bookViews>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">    By age</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Under 18</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">        Over 24 </t>
+  </si>
+  <si>
+    <t>Years</t>
   </si>
 </sst>
 </file>
@@ -82,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,106 +401,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275377FA-8C17-4C67-A95A-BA30635E8CCA}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>2015</v>
       </c>
-      <c r="C1">
+      <c r="B2" s="1">
+        <v>127787</v>
+      </c>
+      <c r="C2" s="1">
+        <v>52973</v>
+      </c>
+      <c r="D2" s="1">
+        <v>383948</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2016</v>
       </c>
-      <c r="D1">
+      <c r="B3" s="1">
+        <v>120819</v>
+      </c>
+      <c r="C3" s="1">
+        <v>50001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>379108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2017</v>
       </c>
-      <c r="E1">
+      <c r="B4" s="1">
+        <v>114529</v>
+      </c>
+      <c r="C4" s="1">
+        <v>50992</v>
+      </c>
+      <c r="D4" s="1">
+        <v>385475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2018</v>
       </c>
-      <c r="F1">
+      <c r="B5" s="1">
+        <v>111592</v>
+      </c>
+      <c r="C5" s="1">
+        <v>48319</v>
+      </c>
+      <c r="D5" s="1">
+        <v>392919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>2019</v>
       </c>
-      <c r="G1">
+      <c r="B6" s="1">
+        <v>107069</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45629</v>
+      </c>
+      <c r="D6" s="1">
+        <v>415017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>2020</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>127787</v>
-      </c>
-      <c r="C2">
-        <v>120819</v>
-      </c>
-      <c r="D2">
-        <v>114529</v>
-      </c>
-      <c r="E2">
-        <v>111592</v>
-      </c>
-      <c r="F2">
-        <v>107069</v>
-      </c>
-      <c r="G2">
+      <c r="B7" s="1">
         <v>106364</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>52973</v>
-      </c>
-      <c r="C3">
-        <v>50001</v>
-      </c>
-      <c r="D3">
-        <v>50992</v>
-      </c>
-      <c r="E3">
-        <v>48319</v>
-      </c>
-      <c r="F3">
-        <v>45629</v>
-      </c>
-      <c r="G3">
+      <c r="C7" s="1">
         <v>45243</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>383948</v>
-      </c>
-      <c r="C4">
-        <v>379108</v>
-      </c>
-      <c r="D4">
-        <v>385475</v>
-      </c>
-      <c r="E4">
-        <v>392919</v>
-      </c>
-      <c r="F4">
-        <v>415017</v>
-      </c>
-      <c r="G4">
+      <c r="D7" s="1">
         <v>428859</v>
       </c>
     </row>

</xml_diff>